<commit_message>
Reduced code duplication in SavingsCalculation
</commit_message>
<xml_diff>
--- a/IDP/GenC IDP Product Backlog.xlsx
+++ b/IDP/GenC IDP Product Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARIJIT\Documents\CSDTraining\IDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635A3462-B837-4662-8372-97EE1DFADA07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B628E59-6A4E-460C-8D06-9EA1429AD30D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="5170" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="5170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="7" r:id="rId1"/>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="167">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -665,6 +665,21 @@
   </si>
   <si>
     <t>Write Junit tests for Category  controller</t>
+  </si>
+  <si>
+    <t>User Story #6</t>
+  </si>
+  <si>
+    <t>User Story #7</t>
+  </si>
+  <si>
+    <t>User Story #8</t>
+  </si>
+  <si>
+    <t>User Story #9</t>
+  </si>
+  <si>
+    <t>User Story #10</t>
   </si>
 </sst>
 </file>
@@ -1699,6 +1714,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="145" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="145" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1715,9 +1733,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="145" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="146">
@@ -3712,7 +3727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H34"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -3984,7 +3999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView topLeftCell="C8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -4215,9 +4230,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="11.5" x14ac:dyDescent="0.35"/>
@@ -4308,7 +4323,7 @@
       <c r="B4" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="108" t="s">
+      <c r="C4" s="99" t="s">
         <v>58</v>
       </c>
       <c r="D4" s="60"/>
@@ -4327,7 +4342,7 @@
       <c r="B5" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="99"/>
+      <c r="C5" s="100"/>
       <c r="D5" s="53" t="s">
         <v>73</v>
       </c>
@@ -4360,7 +4375,7 @@
       <c r="B6" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="99"/>
+      <c r="C6" s="100"/>
       <c r="D6" s="53" t="s">
         <v>74</v>
       </c>
@@ -4393,7 +4408,7 @@
       <c r="B7" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="99"/>
+      <c r="C7" s="100"/>
       <c r="D7" s="53" t="s">
         <v>75</v>
       </c>
@@ -4426,7 +4441,7 @@
       <c r="B8" s="69" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="100"/>
+      <c r="C8" s="101"/>
       <c r="D8" s="53" t="s">
         <v>76</v>
       </c>
@@ -4459,7 +4474,7 @@
       <c r="B9" s="70" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="108" t="s">
+      <c r="C9" s="99" t="s">
         <v>58</v>
       </c>
     </row>
@@ -4470,7 +4485,7 @@
       <c r="B10" s="69" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="99"/>
+      <c r="C10" s="100"/>
       <c r="D10" s="53" t="s">
         <v>126</v>
       </c>
@@ -4503,7 +4518,7 @@
       <c r="B11" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="99"/>
+      <c r="C11" s="100"/>
       <c r="D11" s="53" t="s">
         <v>127</v>
       </c>
@@ -4536,7 +4551,7 @@
       <c r="B12" s="69" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="99"/>
+      <c r="C12" s="100"/>
       <c r="D12" s="53" t="s">
         <v>128</v>
       </c>
@@ -4569,7 +4584,7 @@
       <c r="B13" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="C13" s="100"/>
+      <c r="C13" s="101"/>
       <c r="D13" s="53" t="s">
         <v>129</v>
       </c>
@@ -4602,7 +4617,7 @@
       <c r="B14" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="108" t="s">
+      <c r="C14" s="99" t="s">
         <v>58</v>
       </c>
       <c r="I14" s="57"/>
@@ -4614,7 +4629,7 @@
       <c r="B15" s="69" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="99"/>
+      <c r="C15" s="100"/>
       <c r="D15" s="53" t="s">
         <v>130</v>
       </c>
@@ -4647,7 +4662,7 @@
       <c r="B16" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="99"/>
+      <c r="C16" s="100"/>
       <c r="D16" s="53" t="s">
         <v>131</v>
       </c>
@@ -4680,7 +4695,7 @@
       <c r="B17" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="99"/>
+      <c r="C17" s="100"/>
       <c r="D17" s="53" t="s">
         <v>132</v>
       </c>
@@ -4713,7 +4728,7 @@
       <c r="B18" s="69" t="s">
         <v>89</v>
       </c>
-      <c r="C18" s="100"/>
+      <c r="C18" s="101"/>
       <c r="D18" s="53" t="s">
         <v>133</v>
       </c>
@@ -4746,7 +4761,7 @@
       <c r="B19" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="108" t="s">
+      <c r="C19" s="99" t="s">
         <v>58</v>
       </c>
     </row>
@@ -4757,7 +4772,7 @@
       <c r="B20" s="69" t="s">
         <v>92</v>
       </c>
-      <c r="C20" s="99"/>
+      <c r="C20" s="100"/>
       <c r="D20" s="53" t="s">
         <v>134</v>
       </c>
@@ -4790,7 +4805,7 @@
       <c r="B21" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="C21" s="99"/>
+      <c r="C21" s="100"/>
       <c r="D21" s="53" t="s">
         <v>135</v>
       </c>
@@ -4823,7 +4838,7 @@
       <c r="B22" s="69" t="s">
         <v>136</v>
       </c>
-      <c r="C22" s="99"/>
+      <c r="C22" s="100"/>
       <c r="D22" s="53" t="s">
         <v>137</v>
       </c>
@@ -4856,7 +4871,7 @@
       <c r="B23" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="100"/>
+      <c r="C23" s="101"/>
       <c r="D23" s="53" t="s">
         <v>138</v>
       </c>
@@ -4889,7 +4904,7 @@
       <c r="B24" s="70" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="108" t="s">
+      <c r="C24" s="99" t="s">
         <v>58</v>
       </c>
     </row>
@@ -4900,7 +4915,7 @@
       <c r="B25" s="69" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="99"/>
+      <c r="C25" s="100"/>
       <c r="D25" s="53" t="s">
         <v>139</v>
       </c>
@@ -4933,7 +4948,7 @@
       <c r="B26" s="69" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="99"/>
+      <c r="C26" s="100"/>
       <c r="D26" s="53" t="s">
         <v>140</v>
       </c>
@@ -4966,7 +4981,7 @@
       <c r="B27" s="69" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="99"/>
+      <c r="C27" s="100"/>
       <c r="D27" s="53" t="s">
         <v>141</v>
       </c>
@@ -4999,7 +5014,7 @@
       <c r="B28" s="69" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="100"/>
+      <c r="C28" s="101"/>
       <c r="D28" s="53" t="s">
         <v>139</v>
       </c>
@@ -5027,12 +5042,12 @@
     </row>
     <row r="29" spans="1:11" ht="26" x14ac:dyDescent="0.35">
       <c r="A29" s="70" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="B29" s="70" t="s">
         <v>101</v>
       </c>
-      <c r="C29" s="108" t="s">
+      <c r="C29" s="99" t="s">
         <v>58</v>
       </c>
     </row>
@@ -5043,7 +5058,7 @@
       <c r="B30" s="69" t="s">
         <v>102</v>
       </c>
-      <c r="C30" s="99"/>
+      <c r="C30" s="100"/>
       <c r="D30" s="53" t="s">
         <v>142</v>
       </c>
@@ -5076,7 +5091,7 @@
       <c r="B31" s="69" t="s">
         <v>103</v>
       </c>
-      <c r="C31" s="99"/>
+      <c r="C31" s="100"/>
       <c r="D31" s="53" t="s">
         <v>143</v>
       </c>
@@ -5109,7 +5124,7 @@
       <c r="B32" s="69" t="s">
         <v>104</v>
       </c>
-      <c r="C32" s="99"/>
+      <c r="C32" s="100"/>
       <c r="D32" s="53" t="s">
         <v>144</v>
       </c>
@@ -5142,7 +5157,7 @@
       <c r="B33" s="69" t="s">
         <v>105</v>
       </c>
-      <c r="C33" s="100"/>
+      <c r="C33" s="101"/>
       <c r="D33" s="53" t="s">
         <v>145</v>
       </c>
@@ -5170,12 +5185,12 @@
     </row>
     <row r="34" spans="1:11" ht="26" x14ac:dyDescent="0.35">
       <c r="A34" s="70" t="s">
-        <v>78</v>
+        <v>163</v>
       </c>
       <c r="B34" s="70" t="s">
         <v>106</v>
       </c>
-      <c r="C34" s="108" t="s">
+      <c r="C34" s="99" t="s">
         <v>58</v>
       </c>
     </row>
@@ -5186,7 +5201,7 @@
       <c r="B35" s="69" t="s">
         <v>107</v>
       </c>
-      <c r="C35" s="99"/>
+      <c r="C35" s="100"/>
       <c r="D35" s="53" t="s">
         <v>146</v>
       </c>
@@ -5219,7 +5234,7 @@
       <c r="B36" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="C36" s="99"/>
+      <c r="C36" s="100"/>
       <c r="D36" s="53" t="s">
         <v>147</v>
       </c>
@@ -5252,7 +5267,7 @@
       <c r="B37" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="99"/>
+      <c r="C37" s="100"/>
       <c r="D37" s="53" t="s">
         <v>148</v>
       </c>
@@ -5285,7 +5300,7 @@
       <c r="B38" s="69" t="s">
         <v>110</v>
       </c>
-      <c r="C38" s="100"/>
+      <c r="C38" s="101"/>
       <c r="D38" s="53" t="s">
         <v>149</v>
       </c>
@@ -5313,12 +5328,12 @@
     </row>
     <row r="39" spans="1:11" ht="26" x14ac:dyDescent="0.35">
       <c r="A39" s="70" t="s">
-        <v>84</v>
+        <v>164</v>
       </c>
       <c r="B39" s="70" t="s">
         <v>111</v>
       </c>
-      <c r="C39" s="108" t="s">
+      <c r="C39" s="99" t="s">
         <v>58</v>
       </c>
     </row>
@@ -5329,7 +5344,7 @@
       <c r="B40" s="69" t="s">
         <v>112</v>
       </c>
-      <c r="C40" s="99"/>
+      <c r="C40" s="100"/>
       <c r="D40" s="53" t="s">
         <v>150</v>
       </c>
@@ -5362,7 +5377,7 @@
       <c r="B41" s="69" t="s">
         <v>113</v>
       </c>
-      <c r="C41" s="99"/>
+      <c r="C41" s="100"/>
       <c r="D41" s="53" t="s">
         <v>151</v>
       </c>
@@ -5395,7 +5410,7 @@
       <c r="B42" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="C42" s="99"/>
+      <c r="C42" s="100"/>
       <c r="D42" s="53" t="s">
         <v>152</v>
       </c>
@@ -5428,7 +5443,7 @@
       <c r="B43" s="69" t="s">
         <v>115</v>
       </c>
-      <c r="C43" s="100"/>
+      <c r="C43" s="101"/>
       <c r="D43" s="53" t="s">
         <v>153</v>
       </c>
@@ -5456,12 +5471,12 @@
     </row>
     <row r="44" spans="1:11" ht="26" x14ac:dyDescent="0.35">
       <c r="A44" s="70" t="s">
-        <v>90</v>
+        <v>165</v>
       </c>
       <c r="B44" s="70" t="s">
         <v>116</v>
       </c>
-      <c r="C44" s="108" t="s">
+      <c r="C44" s="99" t="s">
         <v>58</v>
       </c>
     </row>
@@ -5472,7 +5487,7 @@
       <c r="B45" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="C45" s="99"/>
+      <c r="C45" s="100"/>
       <c r="D45" s="53" t="s">
         <v>154</v>
       </c>
@@ -5505,7 +5520,7 @@
       <c r="B46" s="69" t="s">
         <v>155</v>
       </c>
-      <c r="C46" s="99"/>
+      <c r="C46" s="100"/>
       <c r="D46" s="53" t="s">
         <v>118</v>
       </c>
@@ -5538,7 +5553,7 @@
       <c r="B47" s="69" t="s">
         <v>119</v>
       </c>
-      <c r="C47" s="99"/>
+      <c r="C47" s="100"/>
       <c r="D47" s="53" t="s">
         <v>156</v>
       </c>
@@ -5571,7 +5586,7 @@
       <c r="B48" s="69" t="s">
         <v>120</v>
       </c>
-      <c r="C48" s="100"/>
+      <c r="C48" s="101"/>
       <c r="D48" s="53" t="s">
         <v>157</v>
       </c>
@@ -5599,12 +5614,12 @@
     </row>
     <row r="49" spans="1:11" ht="26" x14ac:dyDescent="0.35">
       <c r="A49" s="70" t="s">
-        <v>95</v>
+        <v>166</v>
       </c>
       <c r="B49" s="70" t="s">
         <v>121</v>
       </c>
-      <c r="C49" s="108" t="s">
+      <c r="C49" s="99" t="s">
         <v>58</v>
       </c>
     </row>
@@ -5615,7 +5630,7 @@
       <c r="B50" s="69" t="s">
         <v>122</v>
       </c>
-      <c r="C50" s="99"/>
+      <c r="C50" s="100"/>
       <c r="D50" s="53" t="s">
         <v>158</v>
       </c>
@@ -5648,7 +5663,7 @@
       <c r="B51" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="C51" s="99"/>
+      <c r="C51" s="100"/>
       <c r="D51" s="53" t="s">
         <v>159</v>
       </c>
@@ -5681,7 +5696,7 @@
       <c r="B52" s="69" t="s">
         <v>124</v>
       </c>
-      <c r="C52" s="99"/>
+      <c r="C52" s="100"/>
       <c r="D52" s="53" t="s">
         <v>160</v>
       </c>
@@ -5714,7 +5729,7 @@
       <c r="B53" s="69" t="s">
         <v>125</v>
       </c>
-      <c r="C53" s="100"/>
+      <c r="C53" s="101"/>
       <c r="D53" s="53" t="s">
         <v>161</v>
       </c>
@@ -5743,19 +5758,19 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="13">
+    <mergeCell ref="C39:C43"/>
+    <mergeCell ref="C44:C48"/>
+    <mergeCell ref="C49:C53"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="C34:C38"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="C4:C8"/>
     <mergeCell ref="C9:C13"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="C19:C23"/>
-    <mergeCell ref="C24:C28"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="C34:C38"/>
-    <mergeCell ref="C39:C43"/>
-    <mergeCell ref="C44:C48"/>
-    <mergeCell ref="C49:C53"/>
   </mergeCells>
   <conditionalFormatting sqref="A82:G1048576 A54:F81 D5:F10 D19:F19 D24:F24 D20:D23 A5:B53 F29:F53 D11:E14 D15:D18 D25:D53">
     <cfRule type="expression" dxfId="8" priority="11">
@@ -5846,34 +5861,34 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="104" t="s">
+      <c r="A4" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="104"/>
-      <c r="D4" s="104"/>
-      <c r="E4" s="106" t="s">
+      <c r="C4" s="105"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="107" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="101" t="s">
+      <c r="F4" s="102" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="101" t="s">
+      <c r="G4" s="102" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="105"/>
+      <c r="A5" s="106"/>
       <c r="B5" s="51" t="s">
         <v>54</v>
       </c>
@@ -5883,9 +5898,9 @@
       <c r="D5" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="107"/>
-      <c r="F5" s="102"/>
-      <c r="G5" s="102"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="103"/>
+      <c r="G5" s="103"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="48">
@@ -6075,15 +6090,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007A9C735C9F3CD54A948D0AD38DF112BF" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4ed022c10c60e9d9c27ee5a95c8ce3b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eac52b12-2228-488c-9d59-8a93d308b64e" xmlns:ns3="951c5514-b77c-4532-82d5-a05f2f7d58e2" xmlns:ns4="3c35e321-f73a-4dae-ae38-a0459de24735" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c8774e4bcccb30488bd145616ae26a30" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="eac52b12-2228-488c-9d59-8a93d308b64e"/>
@@ -6331,6 +6337,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -6350,14 +6365,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8575168F-6331-41DA-B879-8152475B9854}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41347413-0C59-4DAA-B1B8-A99F4386EC68}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6377,6 +6384,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8575168F-6331-41DA-B879-8152475B9854}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C0C9F9C-98B5-480F-B2D6-CAE7CFAF0133}">
   <ds:schemaRefs>

</xml_diff>